<commit_message>
Added Pistol multipliers to XLSX
</commit_message>
<xml_diff>
--- a/FO4 Armament Base DMG Sheet.xlsx
+++ b/FO4 Armament Base DMG Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwils\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwils\Desktop\Fo4 Weapon Patcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E0DDA5-1262-43E4-B5F3-8380FEF563C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F9E5D7-7276-4F32-8821-72B29DC6C081}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8E93DADA-E940-48A4-B184-08199042EE5E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="94">
   <si>
     <t>Ammo Name</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>Reload Speed Mult</t>
+  </si>
+  <si>
+    <t>Base DMG Pistol Mult</t>
+  </si>
+  <si>
+    <t>Out of Range Pistol Mult</t>
   </si>
 </sst>
 </file>
@@ -761,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24A94B9-389F-43E9-809F-E464D1449F8C}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,11 +782,12 @@
     <col min="5" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,13 +813,19 @@
         <v>89</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -823,7 +836,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E2,F2))</f>
+        <f t="shared" ref="D2:D37" si="0">_xlfn.FLOOR.MATH(PRODUCT(E2,F2))</f>
         <v>62</v>
       </c>
       <c r="E2" s="4">
@@ -838,14 +851,20 @@
       <c r="H2" s="7">
         <v>0.9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>47</v>
       </c>
@@ -856,7 +875,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E3,F3))</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="E3" s="4">
@@ -871,14 +890,20 @@
       <c r="H3" s="7">
         <v>0.89</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -889,7 +914,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E4,F4))</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E4" s="4">
@@ -904,14 +929,20 @@
       <c r="H4" s="7">
         <v>0.8</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -922,7 +953,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E5,F5))</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E5" s="4">
@@ -937,14 +968,20 @@
       <c r="H5" s="7">
         <v>0.75</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
@@ -955,7 +992,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E6,F6))</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E6" s="4">
@@ -970,14 +1007,20 @@
       <c r="H6" s="7">
         <v>0.75</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
@@ -988,7 +1031,7 @@
         <v>46</v>
       </c>
       <c r="D7" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E7,F7))</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E7" s="4">
@@ -1003,14 +1046,20 @@
       <c r="H7" s="7">
         <v>0.75</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -1021,7 +1070,7 @@
         <v>50</v>
       </c>
       <c r="D8" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E8,F8))</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E8" s="4">
@@ -1036,14 +1085,20 @@
       <c r="H8" s="7">
         <v>0.7</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -1054,7 +1109,7 @@
         <v>54</v>
       </c>
       <c r="D9" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E9,F9))</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E9" s="4">
@@ -1069,14 +1124,20 @@
       <c r="H9" s="7">
         <v>0.75</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
@@ -1087,7 +1148,7 @@
         <v>56</v>
       </c>
       <c r="D10" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E10,F10))</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="E10" s="4">
@@ -1102,14 +1163,20 @@
       <c r="H10" s="7">
         <v>0.75</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1120,7 +1187,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E11,F11))</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="E11" s="4">
@@ -1135,14 +1202,20 @@
       <c r="H11" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J11" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1153,7 +1226,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E12,F12))</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E12" s="4">
@@ -1168,14 +1241,20 @@
       <c r="H12" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
@@ -1186,7 +1265,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E13,F13))</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E13" s="4">
@@ -1201,14 +1280,20 @@
       <c r="H13" s="7">
         <v>0.5</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1304,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E14,F14))</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E14" s="4">
@@ -1234,14 +1319,20 @@
       <c r="H14" s="7">
         <v>0.68</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
@@ -1252,7 +1343,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E15,F15))</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="E15" s="4">
@@ -1267,14 +1358,20 @@
       <c r="H15" s="7">
         <v>0.7</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
@@ -1285,7 +1382,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E16,F16))</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="E16" s="4">
@@ -1300,14 +1397,20 @@
       <c r="H16" s="7">
         <v>0.5</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
@@ -1318,7 +1421,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E17,F17))</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E17" s="4">
@@ -1333,14 +1436,20 @@
       <c r="H17" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J17" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -1351,7 +1460,7 @@
         <v>52</v>
       </c>
       <c r="D18" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E18,F18))</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E18" s="4">
@@ -1366,14 +1475,20 @@
       <c r="H18" s="7">
         <v>0.6</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J18" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
@@ -1384,7 +1499,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E19,F19))</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="E19" s="4">
@@ -1399,14 +1514,20 @@
       <c r="H19" s="7">
         <v>0.35</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J19" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -1417,7 +1538,7 @@
         <v>58</v>
       </c>
       <c r="D20" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E20,F20))</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="E20" s="4">
@@ -1432,14 +1553,20 @@
       <c r="H20" s="7">
         <v>0.3</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J20" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J20" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -1450,7 +1577,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E21,F21))</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="E21" s="4">
@@ -1465,14 +1592,20 @@
       <c r="H21" s="7">
         <v>0.8</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J21" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
@@ -1483,7 +1616,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E22,F22))</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="E22" s="4">
@@ -1498,14 +1631,20 @@
       <c r="H22" s="7">
         <v>0.8</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J22" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
@@ -1516,7 +1655,7 @@
         <v>32</v>
       </c>
       <c r="D23" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E23,F23))</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="E23" s="4">
@@ -1531,14 +1670,20 @@
       <c r="H23" s="7">
         <v>0.78</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J23" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>33</v>
       </c>
@@ -1549,7 +1694,7 @@
         <v>34</v>
       </c>
       <c r="D24" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E24,F24))</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="E24" s="4">
@@ -1564,14 +1709,20 @@
       <c r="H24" s="7">
         <v>0.85</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>35</v>
       </c>
@@ -1582,7 +1733,7 @@
         <v>36</v>
       </c>
       <c r="D25" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E25,F25))</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="E25" s="4">
@@ -1597,14 +1748,20 @@
       <c r="H25" s="7">
         <v>0.78</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J25" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J25" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1615,7 +1772,7 @@
         <v>38</v>
       </c>
       <c r="D26" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E26,F26))</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="E26" s="4">
@@ -1630,14 +1787,20 @@
       <c r="H26" s="7">
         <v>0.78</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J26" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>62</v>
       </c>
@@ -1648,7 +1811,7 @@
         <v>67</v>
       </c>
       <c r="D27" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E27,F27))</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E27" s="4">
@@ -1663,14 +1826,20 @@
       <c r="H27" s="7">
         <v>0.68</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J27" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>63</v>
       </c>
@@ -1681,7 +1850,7 @@
         <v>66</v>
       </c>
       <c r="D28" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E28,F28))</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E28" s="4">
@@ -1696,14 +1865,20 @@
       <c r="H28" s="7">
         <v>0.52</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J28" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
@@ -1714,7 +1889,7 @@
         <v>68</v>
       </c>
       <c r="D29" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E29,F29))</f>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="E29" s="4">
@@ -1729,14 +1904,20 @@
       <c r="H29" s="7">
         <v>0.9</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J29" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L29" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>69</v>
       </c>
@@ -1747,7 +1928,7 @@
         <v>70</v>
       </c>
       <c r="D30" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E30,F30))</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="E30" s="4">
@@ -1762,14 +1943,20 @@
       <c r="H30" s="7">
         <v>0.78</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J30" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>72</v>
       </c>
@@ -1780,7 +1967,7 @@
         <v>79</v>
       </c>
       <c r="D31" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E31,F31))</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E31" s="4">
@@ -1795,14 +1982,20 @@
       <c r="H31" s="7">
         <v>0.75</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J31" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>73</v>
       </c>
@@ -1813,7 +2006,7 @@
         <v>80</v>
       </c>
       <c r="D32" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E32,F32))</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="E32" s="4">
@@ -1828,14 +2021,20 @@
       <c r="H32" s="7">
         <v>0.68</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J32" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>74</v>
       </c>
@@ -1846,7 +2045,7 @@
         <v>81</v>
       </c>
       <c r="D33" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E33,F33))</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="E33" s="4">
@@ -1861,14 +2060,20 @@
       <c r="H33" s="7">
         <v>0.8</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J33" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J33" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>75</v>
       </c>
@@ -1879,7 +2084,7 @@
         <v>82</v>
       </c>
       <c r="D34" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E34,F34))</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="E34" s="4">
@@ -1894,14 +2099,20 @@
       <c r="H34" s="7">
         <v>0.8</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J34" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K34" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J34" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L34" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>76</v>
       </c>
@@ -1912,7 +2123,7 @@
         <v>83</v>
       </c>
       <c r="D35" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E35,F35))</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="E35" s="4">
@@ -1927,14 +2138,20 @@
       <c r="H35" s="7">
         <v>0.35</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J35" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J35" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L35" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>77</v>
       </c>
@@ -1945,7 +2162,7 @@
         <v>84</v>
       </c>
       <c r="D36" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E36,F36))</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="E36" s="4">
@@ -1960,14 +2177,20 @@
       <c r="H36" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K36" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J36" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>78</v>
       </c>
@@ -1978,7 +2201,7 @@
         <v>85</v>
       </c>
       <c r="D37" s="8">
-        <f>_xlfn.FLOOR.MATH(PRODUCT(E37,F37))</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="E37" s="4">
@@ -1993,10 +2216,16 @@
       <c r="H37" s="7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="J37" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J37" s="10">
+      <c r="L37" s="10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working weapon and OMOD caliber change patcher. Will now patch ALL WEAP & OMOD records you have in your load order into a new esp
</commit_message>
<xml_diff>
--- a/FO4 Armament Base DMG Sheet.xlsx
+++ b/FO4 Armament Base DMG Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwils\Desktop\Fo4 Weapon Patcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F9E5D7-7276-4F32-8821-72B29DC6C081}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE4DD49-E07B-4AEC-A2CC-B070118C9E21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8E93DADA-E940-48A4-B184-08199042EE5E}"/>
   </bookViews>
@@ -770,7 +770,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,13 +1461,13 @@
       </c>
       <c r="D18" s="8">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4">
         <v>0.66</v>
       </c>
       <c r="F18" s="4">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G18" s="7">
         <v>4</v>

</xml_diff>